<commit_message>
almost complete the whole procedure, need optimize, add some graph and code
</commit_message>
<xml_diff>
--- a/1_Doc/task.xlsx
+++ b/1_Doc/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>bug index</t>
   </si>
@@ -45,10 +45,46 @@
     <t>其实断开连接就能实现类似功能为了方便先不管了</t>
   </si>
   <si>
-    <t>×</t>
-  </si>
-  <si>
     <t>传文件只能成功第一次无法重复传给一个client</t>
+  </si>
+  <si>
+    <t>代码逻辑问题+面向字节的tcp报文使我没法区分边界，我靠给指令加上定长长度信息前缀解决。</t>
+  </si>
+  <si>
+    <t>无法创建文件夹</t>
+  </si>
+  <si>
+    <r>
+      <t>注意！</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Android11+ 限制无法在根目录直接创建文件夹</t>
+    </r>
+  </si>
+  <si>
+    <t>播放音乐调用导致app崩溃</t>
+  </si>
+  <si>
+    <t>与vc++编译器类似，如果函数声明了返回值但实际没有返回的话就会崩溃</t>
+  </si>
+  <si>
+    <t>不能一边播放一边传文件要实现互斥，或者可以接收到的文件先放在临时文件夹，传输完成后再放到Music文件夹</t>
+  </si>
+  <si>
+    <t>server的连接设备列表有残留</t>
+  </si>
+  <si>
+    <t>突然没法接收到音频数据</t>
+  </si>
+  <si>
+    <t>是缓存区没来得及取走的问题，很快就发送完了，但是因为我后面改了逻辑不是一有数据就读走导致，发完之后无法触发信号了然而此时我的代码还在执行别的东西。发现关键是qmessagebox会阻塞线程。</t>
   </si>
 </sst>
 </file>
@@ -56,10 +92,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -90,38 +126,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,95 +218,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,25 +272,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,25 +428,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,127 +446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,6 +463,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -445,25 +490,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -493,6 +525,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -516,67 +563,56 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -586,98 +622,98 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -691,6 +727,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1044,7 +1086,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1103,37 +1145,88 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" ht="20" customHeight="1" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" ht="36" customHeight="1" spans="1:4">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" ht="20" customHeight="1" spans="1:1">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" ht="20" customHeight="1" spans="1:1">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" ht="20" customHeight="1" spans="1:1">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:4">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:4">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:3">
       <c r="A9" s="2"/>
-    </row>
-    <row r="10" ht="20" customHeight="1" spans="1:1">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" ht="20" customHeight="1" spans="1:1">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:2">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" ht="28" customHeight="1" spans="1:1">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" ht="20" customHeight="1" spans="1:1">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" ht="20" customHeight="1" spans="1:1">
-      <c r="A13" s="2"/>
+    <row r="12" ht="20" customHeight="1" spans="1:2">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" ht="64" customHeight="1" spans="1:4">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1" spans="1:1">
       <c r="A14" s="2"/>
@@ -1208,11 +1301,19 @@
       <c r="A37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add identityController module and some INS
</commit_message>
<xml_diff>
--- a/1_Doc/task.xlsx
+++ b/1_Doc/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>bug index</t>
   </si>
@@ -55,6 +55,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>注意！</t>
     </r>
     <r>
@@ -86,6 +93,9 @@
   <si>
     <t>是缓存区没来得及取走的问题，很快就发送完了，但是因为我后面改了逻辑不是一有数据就读走导致，发完之后无法触发信号了然而此时我的代码还在执行别的东西。发现关键是qmessagebox会阻塞线程。</t>
   </si>
+  <si>
+    <t>host下发指令有较大延时误差，无法同步播放</t>
+  </si>
 </sst>
 </file>
 
@@ -94,8 +104,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -112,6 +122,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -121,6 +139,74 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,82 +220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -218,9 +228,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,7 +245,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,21 +253,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,187 +282,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,11 +476,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,17 +502,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,22 +525,25 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,9 +565,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -571,149 +581,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -728,9 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1086,7 +1093,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1155,7 +1162,7 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
@@ -1169,7 +1176,7 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
@@ -1183,7 +1190,7 @@
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
@@ -1192,8 +1199,7 @@
     </row>
     <row r="9" ht="20" customHeight="1" spans="1:3">
       <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" ht="20" customHeight="1" spans="1:2">
       <c r="A10" s="2">
@@ -1221,15 +1227,20 @@
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" ht="20" customHeight="1" spans="1:1">
-      <c r="A14" s="2"/>
+    <row r="14" ht="20" customHeight="1" spans="1:2">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1" spans="1:1">
       <c r="A15" s="2"/>

</xml_diff>

<commit_message>
fix bugs, add funcs
</commit_message>
<xml_diff>
--- a/1_Doc/task.xlsx
+++ b/1_Doc/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>bug index</t>
   </si>
@@ -96,16 +96,19 @@
   <si>
     <t>host下发指令有较大延时误差，无法同步播放</t>
   </si>
+  <si>
+    <t>连续发送文件时，无法分割当前接收的文件与下一条指令</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -122,16 +125,30 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,8 +161,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,34 +176,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -228,24 +239,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,145 +285,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,36 +466,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,21 +476,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -502,6 +490,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,7 +528,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,7 +537,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,21 +562,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,145 +584,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1093,7 +1096,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1242,8 +1245,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" ht="20" customHeight="1" spans="1:1">
-      <c r="A15" s="2"/>
+    <row r="15" ht="46" customHeight="1" spans="1:2">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1" spans="1:1">
       <c r="A16" s="2"/>

</xml_diff>

<commit_message>
fix the bug that push prebtn will cause client can't normally play next song
</commit_message>
<xml_diff>
--- a/1_Doc/task.xlsx
+++ b/1_Doc/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>bug index</t>
   </si>
@@ -130,7 +130,7 @@
     <t>在某种情况下server的播放与暂停与client刚好是相反的。</t>
   </si>
   <si>
-    <t>实在按上一曲的之后会操作导致相反，如果按发送重播指令正常</t>
+    <t>实在按上一曲的之后会操作导致相反，如果按发送重播指令正常，通过将上一曲的指令改为setsource+playback直接播放而不是replay后问题解决，我觉得可能是player setSource之后本来就没再播放状态，此时调用stop可能会出问题。</t>
   </si>
   <si>
     <t>server端拖动进度条会被弹回去而client端已经拖动成功</t>
@@ -1152,8 +1152,8 @@
   <sheetPr/>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1372,7 +1372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" ht="36" customHeight="1" spans="1:3">
+    <row r="20" ht="82" customHeight="1" spans="1:4">
       <c r="A20" s="2">
         <v>15</v>
       </c>
@@ -1381,6 +1381,9 @@
       </c>
       <c r="C20" s="7" t="s">
         <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" ht="40" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
change a sync method
</commit_message>
<xml_diff>
--- a/1_Doc/task.xlsx
+++ b/1_Doc/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>bug index</t>
   </si>
@@ -130,7 +130,7 @@
     <t>在某种情况下server的播放与暂停与client刚好是相反的。</t>
   </si>
   <si>
-    <t>实在按上一曲的之后会操作导致相反，如果按发送重播指令正常，通过将上一曲的指令改为setsource+playback直接播放而不是replay后问题解决，我觉得可能是player setSource之后本来就没再播放状态，此时调用stop可能会出问题。</t>
+    <t>实在按上一曲的之后会操作导致相反，如果按发送重播指令正常，通过将上一曲的指令改为setsource+playback直接播放而不是replay后问题解决，我觉得可能是player setSource之后本来就没再播放状态，此时调用stop可能会出问题。不对，根本原因不在这，应该还是指令堆积在了缓冲里没来得及取出来。。。。</t>
   </si>
   <si>
     <t>server端拖动进度条会被弹回去而client端已经拖动成功</t>
@@ -1152,8 +1152,8 @@
   <sheetPr/>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1372,7 +1372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" ht="82" customHeight="1" spans="1:4">
+    <row r="20" ht="123" customHeight="1" spans="1:3">
       <c r="A20" s="2">
         <v>15</v>
       </c>
@@ -1381,9 +1381,6 @@
       </c>
       <c r="C20" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="21" ht="40" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
fix the main bug, the project can reluctantly run through the process
</commit_message>
<xml_diff>
--- a/1_Doc/task.xlsx
+++ b/1_Doc/task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30048" windowHeight="13620"/>
+    <workbookView windowWidth="16608" windowHeight="27060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>bug index</t>
   </si>
@@ -112,9 +112,6 @@
     <t>lambda capture surrounding variables的时候如果是&amp;那么好像传的是地址，而非引用？换成=就好了。</t>
   </si>
   <si>
-    <t>为什么client的delayTime比server端的还要长？</t>
-  </si>
-  <si>
     <t>Qtimer即使设置了singleshot依然被多次执行</t>
   </si>
   <si>
@@ -143,6 +140,18 @@
   </si>
   <si>
     <t>有easy一点的解决办法，将slider的setTracking设为false就只会在释放滑块时触发信号，现在用的这个乞丐办法。</t>
+  </si>
+  <si>
+    <t>两台设备发送延时是相同的。。这个不对</t>
+  </si>
+  <si>
+    <t>指令时间戳与延时的生成应该放在发送指令的时候，不然就是一样的时间</t>
+  </si>
+  <si>
+    <t>分配5.1立体声的右方声道会崩溃</t>
+  </si>
+  <si>
+    <t>数组越界了，m_lastId只开到了6也就是目前设置的最大id数，但声道是有8个的，所以这里应与声道数保持一致</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1159,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1336,83 +1345,98 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" ht="20" customHeight="1" spans="1:2">
+    <row r="17" ht="34" customHeight="1" spans="1:4">
       <c r="A17" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" ht="34" customHeight="1" spans="1:4">
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:4">
       <c r="A18" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" ht="20" customHeight="1" spans="1:4">
+    <row r="19" ht="123" customHeight="1" spans="1:3">
       <c r="A19" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" ht="40" customHeight="1" spans="1:4">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" ht="123" customHeight="1" spans="1:3">
-      <c r="A20" s="2">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" ht="40" customHeight="1" spans="1:4">
+    <row r="21" ht="83" customHeight="1" spans="1:4">
       <c r="A21" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" ht="83" customHeight="1" spans="1:4">
+    <row r="22" ht="59" customHeight="1" spans="1:4">
       <c r="A22" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" ht="20" customHeight="1" spans="1:1">
+    <row r="23" ht="43" customHeight="1" spans="1:4">
       <c r="A23" s="2"/>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1" spans="1:1">
       <c r="A24" s="2"/>
@@ -1446,9 +1470,6 @@
     </row>
     <row r="34" ht="20" customHeight="1" spans="1:1">
       <c r="A34" s="2"/>
-    </row>
-    <row r="35" ht="20" customHeight="1" spans="1:1">
-      <c r="A35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>